<commit_message>
First Commit by Amandeep
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/ExcelData.xlsx
+++ b/src/test/resources/ExcelData/ExcelData.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bassa\eclipse-workspace\CucumberJavaProject\src\test\resources\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bassa\eclipse-workspace\Team18_LMSProject\src\test\resources\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16B3B7F-434A-45F5-B0ED-E403C4C42153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2CD434-E175-41EF-B0C9-F4ED015B84F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20895" yWindow="-17715" windowWidth="17280" windowHeight="8925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Register" sheetId="2" r:id="rId2"/>
-    <sheet name="PythonCode" sheetId="3" r:id="rId3"/>
+    <sheet name="User" sheetId="4" r:id="rId2"/>
+    <sheet name="Program" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>username</t>
   </si>
@@ -35,112 +35,12 @@
   <si>
     <t>Project321@</t>
   </si>
-  <si>
-    <t>confirmpassword</t>
-  </si>
-  <si>
-    <t>dsalgoproject811</t>
-  </si>
-  <si>
-    <t>pythonCode</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>print("hello World");</t>
-  </si>
-  <si>
-    <t>hello</t>
-  </si>
-  <si>
-    <t>hello cool cukes</t>
-  </si>
-  <si>
-    <t>def search(input_list, num):
-if(num in input_list):
-print("Element Found")
-\b
-\b
-else:
-print("Not Found")
-\b
-\b
-\b
-\b
-search([12, 23, 45, 67, 6, 90] , 12)</t>
-  </si>
-  <si>
-    <t>Element Found</t>
-  </si>
-  <si>
-    <t>submission success</t>
-  </si>
-  <si>
-    <t>def findMaxConsecutiveOnes(nums) :
-count = 0
-result = 0
-for i in range(0, len(nums)):
-if (nums[i] == 0):
-count = 0
-\b
-\b
-else:
-count+= 1
-\b
-\b
-result = max(result, count)
-\b
-\b
-print(result)
-\b
-\b
-findMaxConsecutiveOnes([1,0,1,1,0,1])</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>def findNumbers(nums):
-c=0
-for i in nums:
-j=str(i)
-x=len(j)
-if x%2==0:
-c=c+1
-\b
-\b
-\b
-\b
-print c
-return c
-findNumbers([12,345,2,6,7896])</t>
-  </si>
-  <si>
-    <t>def sortedSquares(nums):
-squares_list = []
-for i in range(0, len(nums)):
-square = nums[i] * nums[i];
-squares_list.append(square)
-\b
-\b
-sorted_squares_list = sorted(squares_list)
-print sorted_squares_list;
-return sorted_squares_list;
-sortedSquares([-7,-3,2,3,11])</t>
-  </si>
-  <si>
-    <t>[4, 9, 9, 49, 121]</t>
-  </si>
-  <si>
-    <t>hello World</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -163,35 +63,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -207,16 +90,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -536,17 +414,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -554,7 +432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -571,154 +449,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B93F2A34-1C16-4446-901E-CEC46348C378}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ACE6262-2A69-45EE-A27D-9DB311D5BF43}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4838223-FD37-45B2-86C9-E55EE0D6E92F}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{FC0FABD3-4E12-485E-AE65-AA915D6AD912}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{2E7B3B1A-FD75-461E-8CFD-71EFFD7E1150}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{669D10F0-4DBF-441C-898B-80CEA010B7A1}">
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="243.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
program, excel reader,appconfig and apphook updates
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/ExcelData.xlsx
+++ b/src/test/resources/ExcelData/ExcelData.xlsx
@@ -5,24 +5,37 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bassa\eclipse-workspace\Team18_LMSProject\src\test\resources\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Febi\NumpyNinja\LMS-UI-Hackathon_Apr24\Team18_LMSProject\src\test\resources\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF928C8-BC08-4D6C-A49B-157184584E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D0D613-EDCB-41E4-A2B4-04036BF865DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="User" sheetId="4" r:id="rId2"/>
     <sheet name="Program" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -34,6 +47,21 @@
   </si>
   <si>
     <t>UIHackathon@02</t>
+  </si>
+  <si>
+    <t>testcase</t>
+  </si>
+  <si>
+    <t>programName</t>
+  </si>
+  <si>
+    <t>deleteprogram_01</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>xyz</t>
   </si>
 </sst>
 </file>
@@ -124,9 +152,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -164,7 +192,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -270,7 +298,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -412,7 +440,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -420,37 +448,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{57641102-0281-4B15-A23E-862BAEE09273}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{57641102-0281-4B15-A23E-862BAEE09273}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -462,7 +496,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -470,14 +504,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4838223-FD37-45B2-86C9-E55EE0D6E92F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit changes for Home Page
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/ExcelData.xlsx
+++ b/src/test/resources/ExcelData/ExcelData.xlsx
@@ -8,21 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bassa\eclipse-workspace\Team18_LMSProject\src\test\resources\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF928C8-BC08-4D6C-A49B-157184584E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402800A0-ED29-45D1-817A-36E0E1F09513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="User" sheetId="4" r:id="rId2"/>
-    <sheet name="Program" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>username</t>
   </si>
@@ -30,10 +28,13 @@
     <t>password</t>
   </si>
   <si>
+    <t>UIHackathon@02</t>
+  </si>
+  <si>
     <t>sdetorganizers@gmail.com</t>
   </si>
   <si>
-    <t>UIHackathon@02</t>
+    <t>UIHackathon@021231</t>
   </si>
 </sst>
 </file>
@@ -44,14 +45,6 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -71,6 +64,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,20 +96,23 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{5B345234-E3B0-4E93-A87A-3FCB26CF6257}"/>
-    <cellStyle name="Normal 3" xfId="3" xr:uid="{8DC6C142-BA07-4238-9135-0B0E32F5FC4A}"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{5B345234-E3B0-4E93-A87A-3FCB26CF6257}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{8DC6C142-BA07-4238-9135-0B0E32F5FC4A}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -420,16 +424,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -441,43 +445,25 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{57641102-0281-4B15-A23E-862BAEE09273}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{CE2F8421-78DC-4AF2-9736-346BC74B60A1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ACE6262-2A69-45EE-A27D-9DB311D5BF43}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4838223-FD37-45B2-86C9-E55EE0D6E92F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>